<commit_message>
Scriptie - Deelvraag 4 (Experimenten) - verder gewerkt + begonnen aan Sequence diagram
</commit_message>
<xml_diff>
--- a/Nulmetingen TN feb.xlsx
+++ b/Nulmetingen TN feb.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>TrommelProductieID</t>
   </si>
@@ -46,6 +46,30 @@
   </si>
   <si>
     <t>Totaal (x1000)</t>
+  </si>
+  <si>
+    <t>PersProductie Totaal</t>
+  </si>
+  <si>
+    <t>TrommelProductie Totaal</t>
+  </si>
+  <si>
+    <t>OvenProductie Totaal</t>
+  </si>
+  <si>
+    <t>Totaal Generaal</t>
+  </si>
+  <si>
+    <t>PersProductie Totaal (x1000)</t>
+  </si>
+  <si>
+    <t>TrommelProductie Totaal (x1000)</t>
+  </si>
+  <si>
+    <t>OvenProductie Totaal (x1000)</t>
+  </si>
+  <si>
+    <t>Totaal Generaal (x1000)</t>
   </si>
 </sst>
 </file>
@@ -99,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -117,6 +141,7 @@
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -429,8 +454,8 @@
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -518,7 +543,7 @@
         <v>13354</v>
       </c>
       <c r="E3" s="4">
-        <f>500000/C3</f>
+        <f t="shared" ref="E3:E34" si="0">500000/C3</f>
         <v>176805.27021149447</v>
       </c>
       <c r="F3" s="4">
@@ -566,7 +591,7 @@
         <v>13354</v>
       </c>
       <c r="V3" s="4">
-        <f>500000/T3</f>
+        <f t="shared" ref="V3:V38" si="1">500000/T3</f>
         <v>176805.27021149447</v>
       </c>
       <c r="W3" s="4">
@@ -590,11 +615,11 @@
         <v>13370</v>
       </c>
       <c r="E4" s="4">
-        <f>500000/C4</f>
+        <f t="shared" si="0"/>
         <v>214094.16118121741</v>
       </c>
       <c r="F4" s="4">
-        <f>IF(D4=D3,"",SUMIF(D:D,D4,E:E))</f>
+        <f t="shared" ref="F4:F35" si="2">IF(D4=D3,"",SUMIF(D:D,D4,E:E))</f>
         <v>3425506.5788994799</v>
       </c>
       <c r="G4" s="16">
@@ -632,11 +657,11 @@
         <v>13354</v>
       </c>
       <c r="V4" s="4">
-        <f>500000/T4</f>
+        <f t="shared" si="1"/>
         <v>176805.27021149447</v>
       </c>
       <c r="W4" s="4" t="str">
-        <f>IF(U4=U3,"",SUMIF(U:U,U4,V:V))</f>
+        <f t="shared" ref="W4:W39" si="3">IF(U4=U3,"",SUMIF(U:U,U4,V:V))</f>
         <v/>
       </c>
       <c r="X4" s="9"/>
@@ -652,11 +677,11 @@
         <v>13370</v>
       </c>
       <c r="E5" s="4">
-        <f>500000/C5</f>
+        <f t="shared" si="0"/>
         <v>214094.16118121741</v>
       </c>
       <c r="F5" s="4" t="str">
-        <f>IF(D5=D4,"",SUMIF(D:D,D5,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G5" s="16"/>
@@ -681,7 +706,7 @@
         <v>122454.87741858586</v>
       </c>
       <c r="P5" s="13">
-        <f t="shared" ref="P5:P7" si="0">O5/1000</f>
+        <f t="shared" ref="P5:P7" si="4">O5/1000</f>
         <v>122.45487741858587</v>
       </c>
       <c r="S5">
@@ -694,11 +719,11 @@
         <v>13370</v>
       </c>
       <c r="V5" s="4">
-        <f>500000/T5</f>
+        <f t="shared" si="1"/>
         <v>214094.16118121741</v>
       </c>
       <c r="W5" s="4">
-        <f>IF(U5=U4,"",SUMIF(U:U,U5,V:V))</f>
+        <f t="shared" si="3"/>
         <v>642282.48354365223</v>
       </c>
       <c r="X5" s="9">
@@ -717,11 +742,11 @@
         <v>13370</v>
       </c>
       <c r="E6" s="4">
-        <f>500000/C6</f>
+        <f t="shared" si="0"/>
         <v>214094.16118121741</v>
       </c>
       <c r="F6" s="4" t="str">
-        <f>IF(D6=D5,"",SUMIF(D:D,D6,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G6" s="16"/>
@@ -746,7 +771,7 @@
         <v>176805.27021149447</v>
       </c>
       <c r="P6" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>176.80527021149447</v>
       </c>
       <c r="S6">
@@ -759,11 +784,11 @@
         <v>13370</v>
       </c>
       <c r="V6" s="4">
-        <f>500000/T6</f>
+        <f t="shared" si="1"/>
         <v>214094.16118121741</v>
       </c>
       <c r="W6" s="4" t="str">
-        <f>IF(U6=U5,"",SUMIF(U:U,U6,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X6" s="9"/>
@@ -779,11 +804,11 @@
         <v>13370</v>
       </c>
       <c r="E7" s="4">
-        <f>500000/C7</f>
+        <f t="shared" si="0"/>
         <v>214094.16118121741</v>
       </c>
       <c r="F7" s="4" t="str">
-        <f>IF(D7=D6,"",SUMIF(D:D,D7,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G7" s="16"/>
@@ -808,7 +833,7 @@
         <v>182230.35374556269</v>
       </c>
       <c r="P7" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>182.2303537455627</v>
       </c>
       <c r="S7">
@@ -821,11 +846,11 @@
         <v>13370</v>
       </c>
       <c r="V7" s="4">
-        <f>500000/T7</f>
+        <f t="shared" si="1"/>
         <v>214094.16118121741</v>
       </c>
       <c r="W7" s="4" t="str">
-        <f>IF(U7=U6,"",SUMIF(U:U,U7,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X7" s="9"/>
@@ -841,11 +866,11 @@
         <v>13370</v>
       </c>
       <c r="E8" s="4">
-        <f>500000/C8</f>
+        <f t="shared" si="0"/>
         <v>214094.16118121741</v>
       </c>
       <c r="F8" s="4" t="str">
-        <f>IF(D8=D7,"",SUMIF(D:D,D8,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G8" s="16"/>
@@ -861,11 +886,11 @@
         <v>13373</v>
       </c>
       <c r="V8" s="4">
-        <f>500000/T8</f>
+        <f t="shared" si="1"/>
         <v>61836.762078729327</v>
       </c>
       <c r="W8" s="4">
-        <f>IF(U8=U7,"",SUMIF(U:U,U8,V:V))</f>
+        <f t="shared" si="3"/>
         <v>556530.85870856396</v>
       </c>
       <c r="X8" s="9">
@@ -884,11 +909,11 @@
         <v>13370</v>
       </c>
       <c r="E9" s="4">
-        <f>500000/C9</f>
+        <f t="shared" si="0"/>
         <v>214094.16118121741</v>
       </c>
       <c r="F9" s="4" t="str">
-        <f>IF(D9=D8,"",SUMIF(D:D,D9,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G9" s="16"/>
@@ -902,11 +927,11 @@
         <v>13373</v>
       </c>
       <c r="V9" s="4">
-        <f>500000/T9</f>
+        <f t="shared" si="1"/>
         <v>61836.762078729327</v>
       </c>
       <c r="W9" s="4" t="str">
-        <f>IF(U9=U8,"",SUMIF(U:U,U9,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X9" s="9"/>
@@ -922,11 +947,11 @@
         <v>13370</v>
       </c>
       <c r="E10" s="4">
-        <f>500000/C10</f>
+        <f t="shared" si="0"/>
         <v>214094.16118121741</v>
       </c>
       <c r="F10" s="4" t="str">
-        <f>IF(D10=D9,"",SUMIF(D:D,D10,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G10" s="16"/>
@@ -942,11 +967,11 @@
         <v>13373</v>
       </c>
       <c r="V10" s="4">
-        <f>500000/T10</f>
+        <f t="shared" si="1"/>
         <v>61836.762078729327</v>
       </c>
       <c r="W10" s="4" t="str">
-        <f>IF(U10=U9,"",SUMIF(U:U,U10,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X10" s="9"/>
@@ -962,14 +987,20 @@
         <v>13370</v>
       </c>
       <c r="E11" s="4">
-        <f>500000/C11</f>
+        <f t="shared" si="0"/>
         <v>214094.16118121741</v>
       </c>
       <c r="F11" s="4" t="str">
-        <f>IF(D11=D10,"",SUMIF(D:D,D11,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G11" s="16"/>
+      <c r="H11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="S11">
         <v>28801</v>
       </c>
@@ -980,11 +1011,11 @@
         <v>13373</v>
       </c>
       <c r="V11" s="4">
-        <f>500000/T11</f>
+        <f t="shared" si="1"/>
         <v>61836.762078729327</v>
       </c>
       <c r="W11" s="4" t="str">
-        <f>IF(U11=U10,"",SUMIF(U:U,U11,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X11" s="9"/>
@@ -1000,14 +1031,22 @@
         <v>13370</v>
       </c>
       <c r="E12" s="4">
-        <f>500000/C12</f>
+        <f t="shared" si="0"/>
         <v>214094.16118121741</v>
       </c>
       <c r="F12" s="4" t="str">
-        <f>IF(D12=D11,"",SUMIF(D:D,D12,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G12" s="16"/>
+      <c r="H12" s="17">
+        <f>SUM(O3:O7)</f>
+        <v>931088.23985619959</v>
+      </c>
+      <c r="I12" s="4">
+        <f>H12/1000</f>
+        <v>931.08823985619961</v>
+      </c>
       <c r="S12">
         <v>28802</v>
       </c>
@@ -1018,11 +1057,11 @@
         <v>13373</v>
       </c>
       <c r="V12" s="4">
-        <f>500000/T12</f>
+        <f t="shared" si="1"/>
         <v>61836.762078729327</v>
       </c>
       <c r="W12" s="4" t="str">
-        <f>IF(U12=U11,"",SUMIF(U:U,U12,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X12" s="9"/>
@@ -1038,14 +1077,20 @@
         <v>13370</v>
       </c>
       <c r="E13" s="4">
-        <f>500000/C13</f>
+        <f t="shared" si="0"/>
         <v>214094.16118121741</v>
       </c>
       <c r="F13" s="4" t="str">
-        <f>IF(D13=D12,"",SUMIF(D:D,D13,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G13" s="16"/>
+      <c r="H13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="S13">
         <v>28845</v>
       </c>
@@ -1056,11 +1101,11 @@
         <v>13373</v>
       </c>
       <c r="V13" s="4">
-        <f>500000/T13</f>
+        <f t="shared" si="1"/>
         <v>61836.762078729327</v>
       </c>
       <c r="W13" s="4" t="str">
-        <f>IF(U13=U12,"",SUMIF(U:U,U13,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X13" s="9"/>
@@ -1076,14 +1121,22 @@
         <v>13370</v>
       </c>
       <c r="E14" s="4">
-        <f>500000/C14</f>
+        <f t="shared" si="0"/>
         <v>214094.16118121741</v>
       </c>
       <c r="F14" s="4" t="str">
-        <f>IF(D14=D13,"",SUMIF(D:D,D14,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G14" s="16"/>
+      <c r="H14" s="17">
+        <f>SUM(F3:F139)</f>
+        <v>14842782.477187745</v>
+      </c>
+      <c r="I14" s="4">
+        <f>H14/1000</f>
+        <v>14842.782477187746</v>
+      </c>
       <c r="S14">
         <v>28846</v>
       </c>
@@ -1094,11 +1147,11 @@
         <v>13373</v>
       </c>
       <c r="V14" s="4">
-        <f>500000/T14</f>
+        <f t="shared" si="1"/>
         <v>61836.762078729327</v>
       </c>
       <c r="W14" s="4" t="str">
-        <f>IF(U14=U13,"",SUMIF(U:U,U14,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X14" s="9"/>
@@ -1114,14 +1167,20 @@
         <v>13370</v>
       </c>
       <c r="E15" s="4">
-        <f>500000/C15</f>
+        <f t="shared" si="0"/>
         <v>214094.16118121741</v>
       </c>
       <c r="F15" s="4" t="str">
-        <f>IF(D15=D14,"",SUMIF(D:D,D15,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G15" s="16"/>
+      <c r="H15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="S15">
         <v>28905</v>
       </c>
@@ -1132,11 +1191,11 @@
         <v>13373</v>
       </c>
       <c r="V15" s="4">
-        <f>500000/T15</f>
+        <f t="shared" si="1"/>
         <v>61836.762078729327</v>
       </c>
       <c r="W15" s="4" t="str">
-        <f>IF(U15=U14,"",SUMIF(U:U,U15,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X15" s="9"/>
@@ -1152,14 +1211,22 @@
         <v>13370</v>
       </c>
       <c r="E16" s="4">
-        <f>500000/C16</f>
+        <f t="shared" si="0"/>
         <v>214094.16118121741</v>
       </c>
       <c r="F16" s="4" t="str">
-        <f>IF(D16=D15,"",SUMIF(D:D,D16,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G16" s="16"/>
+      <c r="H16" s="2">
+        <f>SUM(W3:W94)</f>
+        <v>8617544.5443589427</v>
+      </c>
+      <c r="I16" s="5">
+        <f>H16/1000</f>
+        <v>8617.5445443589433</v>
+      </c>
       <c r="S16">
         <v>28906</v>
       </c>
@@ -1170,11 +1237,11 @@
         <v>13373</v>
       </c>
       <c r="V16" s="4">
-        <f>500000/T16</f>
+        <f t="shared" si="1"/>
         <v>61836.762078729327</v>
       </c>
       <c r="W16" s="4" t="str">
-        <f>IF(U16=U15,"",SUMIF(U:U,U16,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X16" s="9"/>
@@ -1190,14 +1257,20 @@
         <v>13370</v>
       </c>
       <c r="E17" s="4">
-        <f>500000/C17</f>
+        <f t="shared" si="0"/>
         <v>214094.16118121741</v>
       </c>
       <c r="F17" s="4" t="str">
-        <f>IF(D17=D16,"",SUMIF(D:D,D17,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G17" s="16"/>
+      <c r="H17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="S17">
         <v>28863</v>
       </c>
@@ -1208,11 +1281,11 @@
         <v>13388</v>
       </c>
       <c r="V17" s="4">
-        <f>500000/T17</f>
+        <f t="shared" si="1"/>
         <v>114155.25114155251</v>
       </c>
       <c r="W17" s="4">
-        <f>IF(U17=U16,"",SUMIF(U:U,U17,V:V))</f>
+        <f t="shared" si="3"/>
         <v>342465.75342465751</v>
       </c>
       <c r="X17" s="9">
@@ -1231,14 +1304,22 @@
         <v>13370</v>
       </c>
       <c r="E18" s="4">
-        <f>500000/C18</f>
+        <f t="shared" si="0"/>
         <v>214094.16118121741</v>
       </c>
       <c r="F18" s="4" t="str">
-        <f>IF(D18=D17,"",SUMIF(D:D,D18,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G18" s="16"/>
+      <c r="H18" s="17">
+        <f>SUM(H12,H14,H16)</f>
+        <v>24391415.26140289</v>
+      </c>
+      <c r="I18" s="4">
+        <f>H18/1000</f>
+        <v>24391.41526140289</v>
+      </c>
       <c r="S18">
         <v>28963</v>
       </c>
@@ -1249,11 +1330,11 @@
         <v>13388</v>
       </c>
       <c r="V18" s="4">
-        <f>500000/T18</f>
+        <f t="shared" si="1"/>
         <v>114155.25114155251</v>
       </c>
       <c r="W18" s="4" t="str">
-        <f>IF(U18=U17,"",SUMIF(U:U,U18,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X18" s="9"/>
@@ -1269,11 +1350,11 @@
         <v>13370</v>
       </c>
       <c r="E19" s="4">
-        <f>500000/C19</f>
+        <f t="shared" si="0"/>
         <v>214094.16118121741</v>
       </c>
       <c r="F19" s="4" t="str">
-        <f>IF(D19=D18,"",SUMIF(D:D,D19,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G19" s="16"/>
@@ -1287,11 +1368,11 @@
         <v>13388</v>
       </c>
       <c r="V19" s="4">
-        <f>500000/T19</f>
+        <f t="shared" si="1"/>
         <v>114155.25114155251</v>
       </c>
       <c r="W19" s="4" t="str">
-        <f>IF(U19=U18,"",SUMIF(U:U,U19,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X19" s="9"/>
@@ -1307,11 +1388,11 @@
         <v>13372</v>
       </c>
       <c r="E20" s="4">
-        <f>500000/C20</f>
+        <f t="shared" si="0"/>
         <v>182230.35374556269</v>
       </c>
       <c r="F20" s="4">
-        <f>IF(D20=D19,"",SUMIF(D:D,D20,E:E))</f>
+        <f t="shared" si="2"/>
         <v>364460.70749112539</v>
       </c>
       <c r="G20" s="16">
@@ -1328,11 +1409,11 @@
         <v>13392</v>
       </c>
       <c r="V20" s="4">
-        <f>500000/T20</f>
+        <f t="shared" si="1"/>
         <v>127226.4631043257</v>
       </c>
       <c r="W20" s="4">
-        <f>IF(U20=U19,"",SUMIF(U:U,U20,V:V))</f>
+        <f t="shared" si="3"/>
         <v>381679.38931297709</v>
       </c>
       <c r="X20" s="9">
@@ -1351,11 +1432,11 @@
         <v>13372</v>
       </c>
       <c r="E21" s="4">
-        <f>500000/C21</f>
+        <f t="shared" si="0"/>
         <v>182230.35374556269</v>
       </c>
       <c r="F21" s="4" t="str">
-        <f>IF(D21=D20,"",SUMIF(D:D,D21,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G21" s="16"/>
@@ -1369,11 +1450,11 @@
         <v>13392</v>
       </c>
       <c r="V21" s="4">
-        <f>500000/T21</f>
+        <f t="shared" si="1"/>
         <v>127226.4631043257</v>
       </c>
       <c r="W21" s="4" t="str">
-        <f>IF(U21=U20,"",SUMIF(U:U,U21,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X21" s="9"/>
@@ -1389,11 +1470,11 @@
         <v>13373</v>
       </c>
       <c r="E22" s="4">
-        <f>500000/C22</f>
+        <f t="shared" si="0"/>
         <v>61836.762078729327</v>
       </c>
       <c r="F22" s="4">
-        <f>IF(D22=D21,"",SUMIF(D:D,D22,E:E))</f>
+        <f t="shared" si="2"/>
         <v>680204.38286602264</v>
       </c>
       <c r="G22" s="16">
@@ -1410,11 +1491,11 @@
         <v>13392</v>
       </c>
       <c r="V22" s="4">
-        <f>500000/T22</f>
+        <f t="shared" si="1"/>
         <v>127226.4631043257</v>
       </c>
       <c r="W22" s="4" t="str">
-        <f>IF(U22=U21,"",SUMIF(U:U,U22,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X22" s="9"/>
@@ -1430,11 +1511,11 @@
         <v>13373</v>
       </c>
       <c r="E23" s="4">
-        <f>500000/C23</f>
+        <f t="shared" si="0"/>
         <v>61836.762078729327</v>
       </c>
       <c r="F23" s="4" t="str">
-        <f>IF(D23=D22,"",SUMIF(D:D,D23,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G23" s="16"/>
@@ -1448,11 +1529,11 @@
         <v>13426</v>
       </c>
       <c r="V23" s="4">
-        <f>500000/T23</f>
+        <f t="shared" si="1"/>
         <v>206537.48985900925</v>
       </c>
       <c r="W23" s="4">
-        <f>IF(U23=U22,"",SUMIF(U:U,U23,V:V))</f>
+        <f t="shared" si="3"/>
         <v>413074.9797180185</v>
       </c>
       <c r="X23" s="9">
@@ -1471,11 +1552,11 @@
         <v>13373</v>
       </c>
       <c r="E24" s="4">
-        <f>500000/C24</f>
+        <f t="shared" si="0"/>
         <v>61836.762078729327</v>
       </c>
       <c r="F24" s="4" t="str">
-        <f>IF(D24=D23,"",SUMIF(D:D,D24,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G24" s="16"/>
@@ -1489,11 +1570,11 @@
         <v>13426</v>
       </c>
       <c r="V24" s="4">
-        <f>500000/T24</f>
+        <f t="shared" si="1"/>
         <v>206537.48985900925</v>
       </c>
       <c r="W24" s="4" t="str">
-        <f>IF(U24=U23,"",SUMIF(U:U,U24,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X24" s="9"/>
@@ -1509,11 +1590,11 @@
         <v>13373</v>
       </c>
       <c r="E25" s="4">
-        <f>500000/C25</f>
+        <f t="shared" si="0"/>
         <v>61836.762078729327</v>
       </c>
       <c r="F25" s="4" t="str">
-        <f>IF(D25=D24,"",SUMIF(D:D,D25,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G25" s="16"/>
@@ -1527,11 +1608,11 @@
         <v>13438</v>
       </c>
       <c r="V25" s="4">
-        <f>500000/T25</f>
+        <f t="shared" si="1"/>
         <v>108950.28794471602</v>
       </c>
       <c r="W25" s="4">
-        <f>IF(U25=U24,"",SUMIF(U:U,U25,V:V))</f>
+        <f t="shared" si="3"/>
         <v>217900.57588943205</v>
       </c>
       <c r="X25" s="9">
@@ -1550,11 +1631,11 @@
         <v>13373</v>
       </c>
       <c r="E26" s="4">
-        <f>500000/C26</f>
+        <f t="shared" si="0"/>
         <v>61836.762078729327</v>
       </c>
       <c r="F26" s="4" t="str">
-        <f>IF(D26=D25,"",SUMIF(D:D,D26,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G26" s="16"/>
@@ -1568,11 +1649,11 @@
         <v>13438</v>
       </c>
       <c r="V26" s="4">
-        <f>500000/T26</f>
+        <f t="shared" si="1"/>
         <v>108950.28794471602</v>
       </c>
       <c r="W26" s="4" t="str">
-        <f>IF(U26=U25,"",SUMIF(U:U,U26,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X26" s="9"/>
@@ -1588,11 +1669,11 @@
         <v>13373</v>
       </c>
       <c r="E27" s="4">
-        <f>500000/C27</f>
+        <f t="shared" si="0"/>
         <v>61836.762078729327</v>
       </c>
       <c r="F27" s="4" t="str">
-        <f>IF(D27=D26,"",SUMIF(D:D,D27,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G27" s="16"/>
@@ -1606,11 +1687,11 @@
         <v>13457</v>
       </c>
       <c r="V27" s="4">
-        <f>500000/T27</f>
+        <f t="shared" si="1"/>
         <v>112508.99790710762</v>
       </c>
       <c r="W27" s="4">
-        <f>IF(U27=U26,"",SUMIF(U:U,U27,V:V))</f>
+        <f t="shared" si="3"/>
         <v>225017.99581421525</v>
       </c>
       <c r="X27" s="9">
@@ -1629,11 +1710,11 @@
         <v>13373</v>
       </c>
       <c r="E28" s="4">
-        <f>500000/C28</f>
+        <f t="shared" si="0"/>
         <v>61836.762078729327</v>
       </c>
       <c r="F28" s="4" t="str">
-        <f>IF(D28=D27,"",SUMIF(D:D,D28,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G28" s="16"/>
@@ -1647,11 +1728,11 @@
         <v>13457</v>
       </c>
       <c r="V28" s="4">
-        <f>500000/T28</f>
+        <f t="shared" si="1"/>
         <v>112508.99790710762</v>
       </c>
       <c r="W28" s="4" t="str">
-        <f>IF(U28=U27,"",SUMIF(U:U,U28,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X28" s="9"/>
@@ -1667,11 +1748,11 @@
         <v>13373</v>
       </c>
       <c r="E29" s="4">
-        <f>500000/C29</f>
+        <f t="shared" si="0"/>
         <v>61836.762078729327</v>
       </c>
       <c r="F29" s="4" t="str">
-        <f>IF(D29=D28,"",SUMIF(D:D,D29,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G29" s="16"/>
@@ -1685,11 +1766,11 @@
         <v>13459</v>
       </c>
       <c r="V29" s="4">
-        <f>500000/T29</f>
+        <f t="shared" si="1"/>
         <v>72504.89625564414</v>
       </c>
       <c r="W29" s="4">
-        <f>IF(U29=U28,"",SUMIF(U:U,U29,V:V))</f>
+        <f t="shared" si="3"/>
         <v>652544.06630079728</v>
       </c>
       <c r="X29" s="9">
@@ -1708,11 +1789,11 @@
         <v>13373</v>
       </c>
       <c r="E30" s="4">
-        <f>500000/C30</f>
+        <f t="shared" si="0"/>
         <v>61836.762078729327</v>
       </c>
       <c r="F30" s="4" t="str">
-        <f>IF(D30=D29,"",SUMIF(D:D,D30,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G30" s="16"/>
@@ -1726,11 +1807,11 @@
         <v>13459</v>
       </c>
       <c r="V30" s="4">
-        <f>500000/T30</f>
+        <f t="shared" si="1"/>
         <v>72504.89625564414</v>
       </c>
       <c r="W30" s="4" t="str">
-        <f>IF(U30=U29,"",SUMIF(U:U,U30,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1745,11 +1826,11 @@
         <v>13373</v>
       </c>
       <c r="E31" s="4">
-        <f>500000/C31</f>
+        <f t="shared" si="0"/>
         <v>61836.762078729327</v>
       </c>
       <c r="F31" s="4" t="str">
-        <f>IF(D31=D30,"",SUMIF(D:D,D31,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G31" s="16"/>
@@ -1763,11 +1844,11 @@
         <v>13459</v>
       </c>
       <c r="V31" s="4">
-        <f>500000/T31</f>
+        <f t="shared" si="1"/>
         <v>72504.89625564414</v>
       </c>
       <c r="W31" s="4" t="str">
-        <f>IF(U31=U30,"",SUMIF(U:U,U31,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X31" s="9"/>
@@ -1783,11 +1864,11 @@
         <v>13373</v>
       </c>
       <c r="E32" s="4">
-        <f>500000/C32</f>
+        <f t="shared" si="0"/>
         <v>61836.762078729327</v>
       </c>
       <c r="F32" s="4" t="str">
-        <f>IF(D32=D31,"",SUMIF(D:D,D32,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G32" s="16"/>
@@ -1801,11 +1882,11 @@
         <v>13459</v>
       </c>
       <c r="V32" s="4">
-        <f>500000/T32</f>
+        <f t="shared" si="1"/>
         <v>72504.89625564414</v>
       </c>
       <c r="W32" s="4" t="str">
-        <f>IF(U32=U31,"",SUMIF(U:U,U32,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X32" s="9"/>
@@ -1821,11 +1902,11 @@
         <v>13388</v>
       </c>
       <c r="E33" s="4">
-        <f>500000/C33</f>
+        <f t="shared" si="0"/>
         <v>114155.25114155251</v>
       </c>
       <c r="F33" s="4">
-        <f>IF(D33=D32,"",SUMIF(D:D,D33,E:E))</f>
+        <f t="shared" si="2"/>
         <v>684931.50684931502</v>
       </c>
       <c r="G33" s="16">
@@ -1842,11 +1923,11 @@
         <v>13459</v>
       </c>
       <c r="V33" s="4">
-        <f>500000/T33</f>
+        <f t="shared" si="1"/>
         <v>72504.89625564414</v>
       </c>
       <c r="W33" s="4" t="str">
-        <f>IF(U33=U32,"",SUMIF(U:U,U33,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X33" s="9"/>
@@ -1862,11 +1943,11 @@
         <v>13388</v>
       </c>
       <c r="E34" s="4">
-        <f>500000/C34</f>
+        <f t="shared" si="0"/>
         <v>114155.25114155251</v>
       </c>
       <c r="F34" s="4" t="str">
-        <f>IF(D34=D33,"",SUMIF(D:D,D34,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G34" s="16"/>
@@ -1880,11 +1961,11 @@
         <v>13459</v>
       </c>
       <c r="V34" s="4">
-        <f>500000/T34</f>
+        <f t="shared" si="1"/>
         <v>72504.89625564414</v>
       </c>
       <c r="W34" s="4" t="str">
-        <f>IF(U34=U33,"",SUMIF(U:U,U34,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X34" s="9"/>
@@ -1900,11 +1981,11 @@
         <v>13388</v>
       </c>
       <c r="E35" s="4">
-        <f>500000/C35</f>
+        <f t="shared" ref="E35:E58" si="5">500000/C35</f>
         <v>114155.25114155251</v>
       </c>
       <c r="F35" s="4" t="str">
-        <f>IF(D35=D34,"",SUMIF(D:D,D35,E:E))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G35" s="16"/>
@@ -1918,11 +1999,11 @@
         <v>13459</v>
       </c>
       <c r="V35" s="4">
-        <f>500000/T35</f>
+        <f t="shared" si="1"/>
         <v>72504.89625564414</v>
       </c>
       <c r="W35" s="4" t="str">
-        <f>IF(U35=U34,"",SUMIF(U:U,U35,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X35" s="9"/>
@@ -1938,11 +2019,11 @@
         <v>13388</v>
       </c>
       <c r="E36" s="4">
-        <f>500000/C36</f>
+        <f t="shared" si="5"/>
         <v>114155.25114155251</v>
       </c>
       <c r="F36" s="4" t="str">
-        <f>IF(D36=D35,"",SUMIF(D:D,D36,E:E))</f>
+        <f t="shared" ref="F36:F67" si="6">IF(D36=D35,"",SUMIF(D:D,D36,E:E))</f>
         <v/>
       </c>
       <c r="G36" s="16"/>
@@ -1956,11 +2037,11 @@
         <v>13459</v>
       </c>
       <c r="V36" s="4">
-        <f>500000/T36</f>
+        <f t="shared" si="1"/>
         <v>72504.89625564414</v>
       </c>
       <c r="W36" s="4" t="str">
-        <f>IF(U36=U35,"",SUMIF(U:U,U36,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X36" s="9"/>
@@ -1976,11 +2057,11 @@
         <v>13388</v>
       </c>
       <c r="E37" s="4">
-        <f>500000/C37</f>
+        <f t="shared" si="5"/>
         <v>114155.25114155251</v>
       </c>
       <c r="F37" s="4" t="str">
-        <f>IF(D37=D36,"",SUMIF(D:D,D37,E:E))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G37" s="16"/>
@@ -1994,11 +2075,11 @@
         <v>13459</v>
       </c>
       <c r="V37" s="4">
-        <f>500000/T37</f>
+        <f t="shared" si="1"/>
         <v>72504.89625564414</v>
       </c>
       <c r="W37" s="4" t="str">
-        <f>IF(U37=U36,"",SUMIF(U:U,U37,V:V))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="X37" s="9"/>
@@ -2014,11 +2095,11 @@
         <v>13388</v>
       </c>
       <c r="E38" s="4">
-        <f>500000/C38</f>
+        <f t="shared" si="5"/>
         <v>114155.25114155251</v>
       </c>
       <c r="F38" s="4" t="str">
-        <f>IF(D38=D37,"",SUMIF(D:D,D38,E:E))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G38" s="16"/>
@@ -2032,11 +2113,11 @@
         <v>13471</v>
       </c>
       <c r="V38" s="4">
-        <f>500000/T38</f>
+        <f t="shared" si="1"/>
         <v>104462.75328300319</v>
       </c>
       <c r="W38" s="4">
-        <f>IF(U38=U37,"",SUMIF(U:U,U38,V:V))</f>
+        <f t="shared" si="3"/>
         <v>104462.75328300319</v>
       </c>
       <c r="X38" s="9">
@@ -2055,11 +2136,11 @@
         <v>13392</v>
       </c>
       <c r="E39" s="4">
-        <f>500000/C39</f>
+        <f t="shared" si="5"/>
         <v>127226.4631043257</v>
       </c>
       <c r="F39" s="4">
-        <f>IF(D39=D38,"",SUMIF(D:D,D39,E:E))</f>
+        <f t="shared" si="6"/>
         <v>1017811.7048346056</v>
       </c>
       <c r="G39" s="16">
@@ -2076,11 +2157,11 @@
         <v>13541</v>
       </c>
       <c r="V39" s="4">
-        <f t="shared" ref="V39" si="1">500000/T39</f>
+        <f t="shared" ref="V39" si="7">500000/T39</f>
         <v>20124.190403820056</v>
       </c>
       <c r="W39" s="4">
-        <f>IF(U39=U38,"",SUMIF(U:U,U39,V:V))</f>
+        <f t="shared" si="3"/>
         <v>181117.71363438049</v>
       </c>
       <c r="X39" s="9">
@@ -2099,11 +2180,11 @@
         <v>13392</v>
       </c>
       <c r="E40" s="4">
-        <f>500000/C40</f>
+        <f t="shared" si="5"/>
         <v>127226.4631043257</v>
       </c>
       <c r="F40" s="4" t="str">
-        <f>IF(D40=D39,"",SUMIF(D:D,D40,E:E))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G40" s="16"/>
@@ -2117,7 +2198,7 @@
         <v>13541</v>
       </c>
       <c r="V40" s="4">
-        <f t="shared" ref="V40:V66" si="2">500000/T40</f>
+        <f t="shared" ref="V40:V66" si="8">500000/T40</f>
         <v>20124.190403820056</v>
       </c>
     </row>
@@ -2132,11 +2213,11 @@
         <v>13392</v>
       </c>
       <c r="E41" s="4">
-        <f>500000/C41</f>
+        <f t="shared" si="5"/>
         <v>127226.4631043257</v>
       </c>
       <c r="F41" s="4" t="str">
-        <f>IF(D41=D40,"",SUMIF(D:D,D41,E:E))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G41" s="16"/>
@@ -2150,11 +2231,11 @@
         <v>13541</v>
       </c>
       <c r="V41" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20124.190403820056</v>
       </c>
       <c r="W41" s="4" t="str">
-        <f t="shared" ref="W41:W67" si="3">IF(U41=U40,"",SUMIF(U:U,U41,V:V))</f>
+        <f t="shared" ref="W41:W67" si="9">IF(U41=U40,"",SUMIF(U:U,U41,V:V))</f>
         <v/>
       </c>
       <c r="X41" s="9"/>
@@ -2170,11 +2251,11 @@
         <v>13392</v>
       </c>
       <c r="E42" s="4">
-        <f>500000/C42</f>
+        <f t="shared" si="5"/>
         <v>127226.4631043257</v>
       </c>
       <c r="F42" s="4" t="str">
-        <f>IF(D42=D41,"",SUMIF(D:D,D42,E:E))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G42" s="16"/>
@@ -2188,11 +2269,11 @@
         <v>13541</v>
       </c>
       <c r="V42" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20124.190403820056</v>
       </c>
       <c r="W42" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X42" s="9"/>
@@ -2208,11 +2289,11 @@
         <v>13392</v>
       </c>
       <c r="E43" s="4">
-        <f>500000/C43</f>
+        <f t="shared" si="5"/>
         <v>127226.4631043257</v>
       </c>
       <c r="F43" s="4" t="str">
-        <f>IF(D43=D42,"",SUMIF(D:D,D43,E:E))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G43" s="16"/>
@@ -2226,11 +2307,11 @@
         <v>13541</v>
       </c>
       <c r="V43" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20124.190403820056</v>
       </c>
       <c r="W43" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X43" s="9"/>
@@ -2246,11 +2327,11 @@
         <v>13392</v>
       </c>
       <c r="E44" s="4">
-        <f>500000/C44</f>
+        <f t="shared" si="5"/>
         <v>127226.4631043257</v>
       </c>
       <c r="F44" s="4" t="str">
-        <f>IF(D44=D43,"",SUMIF(D:D,D44,E:E))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G44" s="16"/>
@@ -2264,11 +2345,11 @@
         <v>13541</v>
       </c>
       <c r="V44" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20124.190403820056</v>
       </c>
       <c r="W44" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X44" s="9"/>
@@ -2284,11 +2365,11 @@
         <v>13392</v>
       </c>
       <c r="E45" s="4">
-        <f>500000/C45</f>
+        <f t="shared" si="5"/>
         <v>127226.4631043257</v>
       </c>
       <c r="F45" s="4" t="str">
-        <f>IF(D45=D44,"",SUMIF(D:D,D45,E:E))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G45" s="16"/>
@@ -2302,11 +2383,11 @@
         <v>13541</v>
       </c>
       <c r="V45" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20124.190403820056</v>
       </c>
       <c r="W45" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X45" s="9"/>
@@ -2322,11 +2403,11 @@
         <v>13392</v>
       </c>
       <c r="E46" s="4">
-        <f>500000/C46</f>
+        <f t="shared" si="5"/>
         <v>127226.4631043257</v>
       </c>
       <c r="F46" s="4" t="str">
-        <f>IF(D46=D45,"",SUMIF(D:D,D46,E:E))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G46" s="16"/>
@@ -2340,11 +2421,11 @@
         <v>13541</v>
       </c>
       <c r="V46" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20124.190403820056</v>
       </c>
       <c r="W46" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X46" s="9"/>
@@ -2360,11 +2441,11 @@
         <v>13457</v>
       </c>
       <c r="E47" s="4">
-        <f>500000/C47</f>
+        <f t="shared" si="5"/>
         <v>112508.99790710762</v>
       </c>
       <c r="F47" s="4">
-        <f>IF(D47=D46,"",SUMIF(D:D,D47,E:E))</f>
+        <f t="shared" si="6"/>
         <v>225017.99581421525</v>
       </c>
       <c r="G47" s="16">
@@ -2381,11 +2462,11 @@
         <v>13541</v>
       </c>
       <c r="V47" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20124.190403820056</v>
       </c>
       <c r="W47" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X47" s="9"/>
@@ -2401,11 +2482,11 @@
         <v>13457</v>
       </c>
       <c r="E48" s="4">
-        <f>500000/C48</f>
+        <f t="shared" si="5"/>
         <v>112508.99790710762</v>
       </c>
       <c r="F48" s="4" t="str">
-        <f>IF(D48=D47,"",SUMIF(D:D,D48,E:E))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G48" s="16"/>
@@ -2419,7 +2500,7 @@
         <v>13564</v>
       </c>
       <c r="V48" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>106610.14907297144</v>
       </c>
       <c r="W48" s="4">
@@ -2427,7 +2508,7 @@
         <v>746271.04351080011</v>
       </c>
       <c r="X48" s="9">
-        <f t="shared" ref="X40:X55" si="4">W48/1000</f>
+        <f t="shared" ref="X48:X55" si="10">W48/1000</f>
         <v>746.27104351080015</v>
       </c>
     </row>
@@ -2442,11 +2523,11 @@
         <v>13459</v>
       </c>
       <c r="E49" s="4">
-        <f>500000/C49</f>
+        <f t="shared" si="5"/>
         <v>72504.89625564414</v>
       </c>
       <c r="F49" s="4">
-        <f>IF(D49=D48,"",SUMIF(D:D,D49,E:E))</f>
+        <f t="shared" si="6"/>
         <v>507534.27378950902</v>
       </c>
       <c r="G49" s="16">
@@ -2463,11 +2544,11 @@
         <v>13564</v>
       </c>
       <c r="V49" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>106610.14907297144</v>
       </c>
       <c r="W49" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X49" s="9"/>
@@ -2483,11 +2564,11 @@
         <v>13459</v>
       </c>
       <c r="E50" s="4">
-        <f>500000/C50</f>
+        <f t="shared" si="5"/>
         <v>72504.89625564414</v>
       </c>
       <c r="F50" s="4" t="str">
-        <f>IF(D50=D49,"",SUMIF(D:D,D50,E:E))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G50" s="16"/>
@@ -2501,11 +2582,11 @@
         <v>13564</v>
       </c>
       <c r="V50" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>106610.14907297144</v>
       </c>
       <c r="W50" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X50" s="9"/>
@@ -2521,11 +2602,11 @@
         <v>13459</v>
       </c>
       <c r="E51" s="4">
-        <f>500000/C51</f>
+        <f t="shared" si="5"/>
         <v>72504.89625564414</v>
       </c>
       <c r="F51" s="4" t="str">
-        <f>IF(D51=D50,"",SUMIF(D:D,D51,E:E))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G51" s="16"/>
@@ -2539,11 +2620,11 @@
         <v>13564</v>
       </c>
       <c r="V51" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>106610.14907297144</v>
       </c>
       <c r="W51" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X51" s="9"/>
@@ -2559,11 +2640,11 @@
         <v>13459</v>
       </c>
       <c r="E52" s="4">
-        <f>500000/C52</f>
+        <f t="shared" si="5"/>
         <v>72504.89625564414</v>
       </c>
       <c r="F52" s="4" t="str">
-        <f>IF(D52=D51,"",SUMIF(D:D,D52,E:E))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G52" s="16"/>
@@ -2577,11 +2658,11 @@
         <v>13564</v>
       </c>
       <c r="V52" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>106610.14907297144</v>
       </c>
       <c r="W52" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X52" s="9"/>
@@ -2597,11 +2678,11 @@
         <v>13459</v>
       </c>
       <c r="E53" s="4">
-        <f>500000/C53</f>
+        <f t="shared" si="5"/>
         <v>72504.89625564414</v>
       </c>
       <c r="F53" s="4" t="str">
-        <f>IF(D53=D52,"",SUMIF(D:D,D53,E:E))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G53" s="16"/>
@@ -2615,11 +2696,11 @@
         <v>13564</v>
       </c>
       <c r="V53" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>106610.14907297144</v>
       </c>
       <c r="W53" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X53" s="9"/>
@@ -2635,11 +2716,11 @@
         <v>13459</v>
       </c>
       <c r="E54" s="4">
-        <f>500000/C54</f>
+        <f t="shared" si="5"/>
         <v>72504.89625564414</v>
       </c>
       <c r="F54" s="4" t="str">
-        <f>IF(D54=D53,"",SUMIF(D:D,D54,E:E))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G54" s="16"/>
@@ -2653,11 +2734,11 @@
         <v>13564</v>
       </c>
       <c r="V54" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>106610.14907297144</v>
       </c>
       <c r="W54" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X54" s="9"/>
@@ -2673,11 +2754,11 @@
         <v>13459</v>
       </c>
       <c r="E55" s="4">
-        <f>500000/C55</f>
+        <f t="shared" si="5"/>
         <v>72504.89625564414</v>
       </c>
       <c r="F55" s="4" t="str">
-        <f>IF(D55=D54,"",SUMIF(D:D,D55,E:E))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G55" s="16"/>
@@ -2691,15 +2772,15 @@
         <v>13600</v>
       </c>
       <c r="V55" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20876.879023496509</v>
       </c>
       <c r="W55" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>313153.18535244762</v>
       </c>
       <c r="X55" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>313.15318535244762</v>
       </c>
     </row>
@@ -2714,11 +2795,11 @@
         <v>13464</v>
       </c>
       <c r="E56" s="4">
-        <f>500000/C56</f>
+        <f t="shared" si="5"/>
         <v>24846.83170594868</v>
       </c>
       <c r="F56" s="4">
-        <f>IF(D56=D55,"",SUMIF(D:D,D56,E:E))</f>
+        <f t="shared" si="6"/>
         <v>49693.66341189736</v>
       </c>
       <c r="G56" s="16">
@@ -2735,11 +2816,11 @@
         <v>13600</v>
       </c>
       <c r="V56" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20876.879023496509</v>
       </c>
       <c r="W56" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X56" s="9"/>
@@ -2755,11 +2836,11 @@
         <v>13464</v>
       </c>
       <c r="E57" s="4">
-        <f>500000/C57</f>
+        <f t="shared" si="5"/>
         <v>24846.83170594868</v>
       </c>
       <c r="F57" s="4" t="str">
-        <f>IF(D57=D56,"",SUMIF(D:D,D57,E:E))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G57" s="16"/>
@@ -2773,11 +2854,11 @@
         <v>13600</v>
       </c>
       <c r="V57" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20876.879023496509</v>
       </c>
       <c r="W57" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X57" s="9"/>
@@ -2793,11 +2874,11 @@
         <v>13541</v>
       </c>
       <c r="E58" s="4">
-        <f>500000/C58</f>
+        <f t="shared" si="5"/>
         <v>20124.190403820056</v>
       </c>
       <c r="F58" s="4">
-        <f>IF(D58=D57,"",SUMIF(D:D,D58,E:E))</f>
+        <f t="shared" si="6"/>
         <v>321987.04646112089</v>
       </c>
       <c r="G58" s="16">
@@ -2814,11 +2895,11 @@
         <v>13600</v>
       </c>
       <c r="V58" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20876.879023496509</v>
       </c>
       <c r="W58" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X58" s="9"/>
@@ -2834,7 +2915,7 @@
         <v>13541</v>
       </c>
       <c r="E59" s="4">
-        <f t="shared" ref="E35:E66" si="5">500000/C59</f>
+        <f t="shared" ref="E59:E66" si="11">500000/C59</f>
         <v>20124.190403820056</v>
       </c>
       <c r="F59" s="4"/>
@@ -2848,11 +2929,11 @@
         <v>13600</v>
       </c>
       <c r="V59" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20876.879023496509</v>
       </c>
       <c r="W59" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X59" s="9"/>
@@ -2868,11 +2949,11 @@
         <v>13541</v>
       </c>
       <c r="E60" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>20124.190403820056</v>
       </c>
       <c r="F60" s="4" t="str">
-        <f t="shared" ref="F5:F68" si="6">IF(D60=D59,"",SUMIF(D:D,D60,E:E))</f>
+        <f t="shared" ref="F60:F68" si="12">IF(D60=D59,"",SUMIF(D:D,D60,E:E))</f>
         <v/>
       </c>
       <c r="G60" s="16"/>
@@ -2886,11 +2967,11 @@
         <v>13600</v>
       </c>
       <c r="V60" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20876.879023496509</v>
       </c>
       <c r="W60" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X60" s="9"/>
@@ -2906,11 +2987,11 @@
         <v>13541</v>
       </c>
       <c r="E61" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>20124.190403820056</v>
       </c>
       <c r="F61" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G61" s="16"/>
@@ -2924,11 +3005,11 @@
         <v>13600</v>
       </c>
       <c r="V61" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20876.879023496509</v>
       </c>
       <c r="W61" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X61" s="9"/>
@@ -2944,11 +3025,11 @@
         <v>13541</v>
       </c>
       <c r="E62" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>20124.190403820056</v>
       </c>
       <c r="F62" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G62" s="16"/>
@@ -2962,11 +3043,11 @@
         <v>13600</v>
       </c>
       <c r="V62" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20876.879023496509</v>
       </c>
       <c r="W62" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X62" s="9"/>
@@ -2982,11 +3063,11 @@
         <v>13541</v>
       </c>
       <c r="E63" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>20124.190403820056</v>
       </c>
       <c r="F63" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G63" s="16"/>
@@ -3000,11 +3081,11 @@
         <v>13600</v>
       </c>
       <c r="V63" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20876.879023496509</v>
       </c>
       <c r="W63" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X63" s="9"/>
@@ -3020,11 +3101,11 @@
         <v>13541</v>
       </c>
       <c r="E64" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>20124.190403820056</v>
       </c>
       <c r="F64" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G64" s="16"/>
@@ -3038,11 +3119,11 @@
         <v>13600</v>
       </c>
       <c r="V64" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20876.879023496509</v>
       </c>
       <c r="W64" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X64" s="9"/>
@@ -3058,11 +3139,11 @@
         <v>13541</v>
       </c>
       <c r="E65" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>20124.190403820056</v>
       </c>
       <c r="F65" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G65" s="16"/>
@@ -3076,11 +3157,11 @@
         <v>13600</v>
       </c>
       <c r="V65" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20876.879023496509</v>
       </c>
       <c r="W65" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X65" s="9"/>
@@ -3096,11 +3177,11 @@
         <v>13541</v>
       </c>
       <c r="E66" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>20124.190403820056</v>
       </c>
       <c r="F66" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G66" s="16"/>
@@ -3114,11 +3195,11 @@
         <v>13600</v>
       </c>
       <c r="V66" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20876.879023496509</v>
       </c>
       <c r="W66" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X66" s="9"/>
@@ -3134,11 +3215,11 @@
         <v>13541</v>
       </c>
       <c r="E67" s="4">
-        <f t="shared" ref="E67:E98" si="7">500000/C67</f>
+        <f t="shared" ref="E67:E98" si="13">500000/C67</f>
         <v>20124.190403820056</v>
       </c>
       <c r="F67" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G67" s="16"/>
@@ -3152,11 +3233,11 @@
         <v>13600</v>
       </c>
       <c r="V67" s="4">
-        <f t="shared" ref="V67:V94" si="8">500000/T67</f>
+        <f t="shared" ref="V67:V94" si="14">500000/T67</f>
         <v>20876.879023496509</v>
       </c>
       <c r="W67" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X67" s="9"/>
@@ -3172,11 +3253,11 @@
         <v>13541</v>
       </c>
       <c r="E68" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20124.190403820056</v>
       </c>
       <c r="F68" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G68" s="16"/>
@@ -3190,11 +3271,11 @@
         <v>13600</v>
       </c>
       <c r="V68" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>20876.879023496509</v>
       </c>
       <c r="W68" s="4" t="str">
-        <f t="shared" ref="W68:W94" si="9">IF(U68=U67,"",SUMIF(U:U,U68,V:V))</f>
+        <f t="shared" ref="W68:W94" si="15">IF(U68=U67,"",SUMIF(U:U,U68,V:V))</f>
         <v/>
       </c>
       <c r="X68" s="9"/>
@@ -3210,11 +3291,11 @@
         <v>13541</v>
       </c>
       <c r="E69" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20124.190403820056</v>
       </c>
       <c r="F69" s="4" t="str">
-        <f t="shared" ref="F69:F132" si="10">IF(D69=D68,"",SUMIF(D:D,D69,E:E))</f>
+        <f t="shared" ref="F69:F132" si="16">IF(D69=D68,"",SUMIF(D:D,D69,E:E))</f>
         <v/>
       </c>
       <c r="G69" s="16"/>
@@ -3228,11 +3309,11 @@
         <v>13600</v>
       </c>
       <c r="V69" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>20876.879023496509</v>
       </c>
       <c r="W69" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X69" s="9"/>
@@ -3248,11 +3329,11 @@
         <v>13541</v>
       </c>
       <c r="E70" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20124.190403820056</v>
       </c>
       <c r="F70" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G70" s="16"/>
@@ -3266,15 +3347,15 @@
         <v>13639</v>
       </c>
       <c r="V70" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>154005.60888427557</v>
       </c>
       <c r="W70" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>154005.60888427557</v>
       </c>
       <c r="X70" s="9">
-        <f t="shared" ref="X70:X93" si="11">W70/1000</f>
+        <f t="shared" ref="X70:X93" si="17">W70/1000</f>
         <v>154.00560888427557</v>
       </c>
     </row>
@@ -3289,11 +3370,11 @@
         <v>13541</v>
       </c>
       <c r="E71" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20124.190403820056</v>
       </c>
       <c r="F71" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G71" s="16"/>
@@ -3307,15 +3388,15 @@
         <v>13678</v>
       </c>
       <c r="V71" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>167427.68128734475</v>
       </c>
       <c r="W71" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1004566.0877240686</v>
       </c>
       <c r="X71" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1004.5660877240686</v>
       </c>
     </row>
@@ -3330,11 +3411,11 @@
         <v>13541</v>
       </c>
       <c r="E72" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20124.190403820056</v>
       </c>
       <c r="F72" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G72" s="16"/>
@@ -3348,11 +3429,11 @@
         <v>13678</v>
       </c>
       <c r="V72" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>167427.68128734475</v>
       </c>
       <c r="W72" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X72" s="9"/>
@@ -3368,11 +3449,11 @@
         <v>13541</v>
       </c>
       <c r="E73" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20124.190403820056</v>
       </c>
       <c r="F73" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G73" s="16"/>
@@ -3386,11 +3467,11 @@
         <v>13678</v>
       </c>
       <c r="V73" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>167427.68128734475</v>
       </c>
       <c r="W73" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X73" s="9"/>
@@ -3406,15 +3487,15 @@
         <v>13564</v>
       </c>
       <c r="E74" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>106610.14907297144</v>
       </c>
       <c r="F74" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>639660.89443782868</v>
       </c>
       <c r="G74" s="16">
-        <f t="shared" ref="G74:G128" si="12">F74/1000</f>
+        <f t="shared" ref="G74:G128" si="18">F74/1000</f>
         <v>639.66089443782869</v>
       </c>
       <c r="S74">
@@ -3427,11 +3508,11 @@
         <v>13678</v>
       </c>
       <c r="V74" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>167427.68128734475</v>
       </c>
       <c r="W74" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X74" s="9"/>
@@ -3447,11 +3528,11 @@
         <v>13564</v>
       </c>
       <c r="E75" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>106610.14907297144</v>
       </c>
       <c r="F75" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G75" s="16"/>
@@ -3465,11 +3546,11 @@
         <v>13678</v>
       </c>
       <c r="V75" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>167427.68128734475</v>
       </c>
       <c r="W75" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X75" s="9"/>
@@ -3485,11 +3566,11 @@
         <v>13564</v>
       </c>
       <c r="E76" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>106610.14907297144</v>
       </c>
       <c r="F76" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G76" s="16"/>
@@ -3503,11 +3584,11 @@
         <v>13678</v>
       </c>
       <c r="V76" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>167427.68128734475</v>
       </c>
       <c r="W76" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X76" s="9"/>
@@ -3523,11 +3604,11 @@
         <v>13564</v>
       </c>
       <c r="E77" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>106610.14907297144</v>
       </c>
       <c r="F77" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G77" s="16"/>
@@ -3541,15 +3622,15 @@
         <v>13682</v>
       </c>
       <c r="V77" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>100046.18131729607</v>
       </c>
       <c r="W77" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>200092.36263459214</v>
       </c>
       <c r="X77" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>200.09236263459215</v>
       </c>
     </row>
@@ -3564,11 +3645,11 @@
         <v>13564</v>
       </c>
       <c r="E78" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>106610.14907297144</v>
       </c>
       <c r="F78" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G78" s="16"/>
@@ -3582,11 +3663,11 @@
         <v>13682</v>
       </c>
       <c r="V78" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>100046.18131729607</v>
       </c>
       <c r="W78" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X78" s="9"/>
@@ -3602,11 +3683,11 @@
         <v>13564</v>
       </c>
       <c r="E79" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>106610.14907297144</v>
       </c>
       <c r="F79" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G79" s="16"/>
@@ -3620,15 +3701,15 @@
         <v>13684</v>
       </c>
       <c r="V79" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>204091.46236430979</v>
       </c>
       <c r="W79" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>816365.84945723915</v>
       </c>
       <c r="X79" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>816.36584945723916</v>
       </c>
     </row>
@@ -3643,15 +3724,15 @@
         <v>13600</v>
       </c>
       <c r="E80" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F80" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>459291.33851692331</v>
       </c>
       <c r="G80" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>459.2913385169233</v>
       </c>
       <c r="S80">
@@ -3664,11 +3745,11 @@
         <v>13684</v>
       </c>
       <c r="V80" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>204091.46236430979</v>
       </c>
       <c r="W80" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X80" s="9"/>
@@ -3684,11 +3765,11 @@
         <v>13600</v>
       </c>
       <c r="E81" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F81" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G81" s="16"/>
@@ -3702,11 +3783,11 @@
         <v>13684</v>
       </c>
       <c r="V81" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>204091.46236430979</v>
       </c>
       <c r="W81" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X81" s="9"/>
@@ -3722,11 +3803,11 @@
         <v>13600</v>
       </c>
       <c r="E82" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F82" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G82" s="16"/>
@@ -3740,11 +3821,11 @@
         <v>13684</v>
       </c>
       <c r="V82" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>204091.46236430979</v>
       </c>
       <c r="W82" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X82" s="9"/>
@@ -3760,11 +3841,11 @@
         <v>13600</v>
       </c>
       <c r="E83" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F83" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G83" s="16"/>
@@ -3778,15 +3859,15 @@
         <v>13704</v>
       </c>
       <c r="V83" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>36343.019959586563</v>
       </c>
       <c r="W83" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>145372.07983834625</v>
       </c>
       <c r="X83" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>145.37207983834625</v>
       </c>
     </row>
@@ -3801,11 +3882,11 @@
         <v>13600</v>
       </c>
       <c r="E84" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F84" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G84" s="16"/>
@@ -3819,11 +3900,11 @@
         <v>13704</v>
       </c>
       <c r="V84" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>36343.019959586563</v>
       </c>
       <c r="W84" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X84" s="9"/>
@@ -3839,11 +3920,11 @@
         <v>13600</v>
       </c>
       <c r="E85" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F85" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G85" s="16"/>
@@ -3857,11 +3938,11 @@
         <v>13704</v>
       </c>
       <c r="V85" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>36343.019959586563</v>
       </c>
       <c r="W85" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X85" s="9"/>
@@ -3877,11 +3958,11 @@
         <v>13600</v>
       </c>
       <c r="E86" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F86" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G86" s="16"/>
@@ -3895,11 +3976,11 @@
         <v>13704</v>
       </c>
       <c r="V86" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>36343.019959586563</v>
       </c>
       <c r="W86" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X86" s="9"/>
@@ -3915,11 +3996,11 @@
         <v>13600</v>
       </c>
       <c r="E87" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F87" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G87" s="16"/>
@@ -3933,15 +4014,15 @@
         <v>20404</v>
       </c>
       <c r="V87" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>581395.34883720928</v>
       </c>
       <c r="W87" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>581395.34883720928</v>
       </c>
       <c r="X87" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>581.39534883720933</v>
       </c>
     </row>
@@ -3956,11 +4037,11 @@
         <v>13600</v>
       </c>
       <c r="E88" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F88" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G88" s="16"/>
@@ -3974,15 +4055,15 @@
         <v>20617</v>
       </c>
       <c r="V88" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>101832.99389002037</v>
       </c>
       <c r="W88" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>509164.96945010184</v>
       </c>
       <c r="X88" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>509.16496945010186</v>
       </c>
     </row>
@@ -3997,11 +4078,11 @@
         <v>13600</v>
       </c>
       <c r="E89" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F89" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G89" s="16"/>
@@ -4015,11 +4096,11 @@
         <v>20617</v>
       </c>
       <c r="V89" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>101832.99389002037</v>
       </c>
       <c r="W89" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X89" s="9"/>
@@ -4035,11 +4116,11 @@
         <v>13600</v>
       </c>
       <c r="E90" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F90" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G90" s="16"/>
@@ -4053,11 +4134,11 @@
         <v>20617</v>
       </c>
       <c r="V90" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>101832.99389002037</v>
       </c>
       <c r="W90" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X90" s="9"/>
@@ -4073,11 +4154,11 @@
         <v>13600</v>
       </c>
       <c r="E91" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F91" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G91" s="16"/>
@@ -4091,11 +4172,11 @@
         <v>20617</v>
       </c>
       <c r="V91" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>101832.99389002037</v>
       </c>
       <c r="W91" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X91" s="9"/>
@@ -4111,11 +4192,11 @@
         <v>13600</v>
       </c>
       <c r="E92" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F92" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G92" s="16"/>
@@ -4129,11 +4210,11 @@
         <v>20617</v>
       </c>
       <c r="V92" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>101832.99389002037</v>
       </c>
       <c r="W92" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X92" s="9"/>
@@ -4149,11 +4230,11 @@
         <v>13600</v>
       </c>
       <c r="E93" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F93" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G93" s="16"/>
@@ -4167,15 +4248,15 @@
         <v>25810</v>
       </c>
       <c r="V93" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>38235.449308588373</v>
       </c>
       <c r="W93" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>76470.898617176746</v>
       </c>
       <c r="X93" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>76.470898617176744</v>
       </c>
     </row>
@@ -4190,11 +4271,11 @@
         <v>13600</v>
       </c>
       <c r="E94" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F94" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G94" s="16"/>
@@ -4208,11 +4289,11 @@
         <v>25810</v>
       </c>
       <c r="V94" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>38235.449308588373</v>
       </c>
       <c r="W94" s="2" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X94" s="9"/>
@@ -4228,11 +4309,11 @@
         <v>13600</v>
       </c>
       <c r="E95" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F95" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G95" s="16"/>
@@ -4248,11 +4329,11 @@
         <v>13600</v>
       </c>
       <c r="E96" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F96" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G96" s="16"/>
@@ -4270,11 +4351,11 @@
         <v>13600</v>
       </c>
       <c r="E97" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F97" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G97" s="16"/>
@@ -4291,11 +4372,11 @@
         <v>13600</v>
       </c>
       <c r="E98" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F98" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G98" s="16"/>
@@ -4312,11 +4393,11 @@
         <v>13600</v>
       </c>
       <c r="E99" s="4">
-        <f t="shared" ref="E99:E130" si="13">500000/C99</f>
+        <f t="shared" ref="E99:E130" si="19">500000/C99</f>
         <v>20876.879023496509</v>
       </c>
       <c r="F99" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G99" s="16"/>
@@ -4333,11 +4414,11 @@
         <v>13600</v>
       </c>
       <c r="E100" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F100" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G100" s="16"/>
@@ -4354,11 +4435,11 @@
         <v>13600</v>
       </c>
       <c r="E101" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>20876.879023496509</v>
       </c>
       <c r="F101" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G101" s="16"/>
@@ -4374,15 +4455,15 @@
         <v>13639</v>
       </c>
       <c r="E102" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>154005.60888427557</v>
       </c>
       <c r="F102" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>308011.21776855114</v>
       </c>
       <c r="G102" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>308.01121776855115</v>
       </c>
     </row>
@@ -4397,11 +4478,11 @@
         <v>13639</v>
       </c>
       <c r="E103" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>154005.60888427557</v>
       </c>
       <c r="F103" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G103" s="16"/>
@@ -4417,15 +4498,15 @@
         <v>13678</v>
       </c>
       <c r="E104" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>167427.68128734475</v>
       </c>
       <c r="F104" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>334855.3625746895</v>
       </c>
       <c r="G104" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>334.85536257468948</v>
       </c>
     </row>
@@ -4440,11 +4521,11 @@
         <v>13678</v>
       </c>
       <c r="E105" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>167427.68128734475</v>
       </c>
       <c r="F105" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G105" s="16"/>
@@ -4460,15 +4541,15 @@
         <v>13679</v>
       </c>
       <c r="E106" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>176507.2394444258</v>
       </c>
       <c r="F106" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>176507.2394444258</v>
       </c>
       <c r="G106" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>176.50723944442581</v>
       </c>
     </row>
@@ -4483,15 +4564,15 @@
         <v>13682</v>
       </c>
       <c r="E107" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>100046.18131729607</v>
       </c>
       <c r="F107" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>100046.18131729607</v>
       </c>
       <c r="G107" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>100.04618131729607</v>
       </c>
     </row>
@@ -4506,15 +4587,15 @@
         <v>13684</v>
       </c>
       <c r="E108" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>204091.46236430979</v>
       </c>
       <c r="F108" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>612274.38709292933</v>
       </c>
       <c r="G108" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>612.27438709292937</v>
       </c>
     </row>
@@ -4529,11 +4610,11 @@
         <v>13684</v>
       </c>
       <c r="E109" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>204091.46236430979</v>
       </c>
       <c r="F109" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G109" s="16"/>
@@ -4549,11 +4630,11 @@
         <v>13684</v>
       </c>
       <c r="E110" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>204091.46236430979</v>
       </c>
       <c r="F110" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G110" s="16"/>
@@ -4569,15 +4650,15 @@
         <v>13704</v>
       </c>
       <c r="E111" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>36343.019959586563</v>
       </c>
       <c r="F111" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>72686.039919173127</v>
       </c>
       <c r="G111" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>72.686039919173126</v>
       </c>
     </row>
@@ -4592,11 +4673,11 @@
         <v>13704</v>
       </c>
       <c r="E112" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>36343.019959586563</v>
       </c>
       <c r="F112" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G112" s="16"/>
@@ -4612,15 +4693,15 @@
         <v>13711</v>
       </c>
       <c r="E113" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>25394.245663932554</v>
       </c>
       <c r="F113" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>50788.491327865107</v>
       </c>
       <c r="G113" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>50.78849132786511</v>
       </c>
     </row>
@@ -4635,11 +4716,11 @@
         <v>13711</v>
       </c>
       <c r="E114" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>25394.245663932554</v>
       </c>
       <c r="F114" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G114" s="16"/>
@@ -4655,15 +4736,15 @@
         <v>20346</v>
       </c>
       <c r="E115" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>147579.6930342385</v>
       </c>
       <c r="F115" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1033057.8512396696</v>
       </c>
       <c r="G115" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>1033.0578512396696</v>
       </c>
     </row>
@@ -4678,11 +4759,11 @@
         <v>20346</v>
       </c>
       <c r="E116" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>147579.6930342385</v>
       </c>
       <c r="F116" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G116" s="16"/>
@@ -4698,11 +4779,11 @@
         <v>20346</v>
       </c>
       <c r="E117" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>147579.6930342385</v>
       </c>
       <c r="F117" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G117" s="16"/>
@@ -4718,11 +4799,11 @@
         <v>20346</v>
       </c>
       <c r="E118" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>147579.6930342385</v>
       </c>
       <c r="F118" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G118" s="16"/>
@@ -4738,11 +4819,11 @@
         <v>20346</v>
       </c>
       <c r="E119" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>147579.6930342385</v>
       </c>
       <c r="F119" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G119" s="16"/>
@@ -4758,11 +4839,11 @@
         <v>20346</v>
       </c>
       <c r="E120" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>147579.6930342385</v>
       </c>
       <c r="F120" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G120" s="16"/>
@@ -4778,11 +4859,11 @@
         <v>20346</v>
       </c>
       <c r="E121" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>147579.6930342385</v>
       </c>
       <c r="F121" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G121" s="16"/>
@@ -4798,15 +4879,15 @@
         <v>20404</v>
       </c>
       <c r="E122" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>581395.34883720928</v>
       </c>
       <c r="F122" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>3488372.0930232559</v>
       </c>
       <c r="G122" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>3488.3720930232557</v>
       </c>
     </row>
@@ -4821,11 +4902,11 @@
         <v>20404</v>
       </c>
       <c r="E123" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>581395.34883720928</v>
       </c>
       <c r="F123" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G123" s="16"/>
@@ -4841,11 +4922,11 @@
         <v>20404</v>
       </c>
       <c r="E124" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>581395.34883720928</v>
       </c>
       <c r="F124" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G124" s="16"/>
@@ -4861,11 +4942,11 @@
         <v>20404</v>
       </c>
       <c r="E125" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>581395.34883720928</v>
       </c>
       <c r="F125" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G125" s="16"/>
@@ -4881,11 +4962,11 @@
         <v>20404</v>
       </c>
       <c r="E126" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>581395.34883720928</v>
       </c>
       <c r="F126" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G126" s="16"/>
@@ -4901,11 +4982,11 @@
         <v>20404</v>
       </c>
       <c r="E127" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>581395.34883720928</v>
       </c>
       <c r="F127" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G127" s="16"/>
@@ -4921,15 +5002,15 @@
         <v>25774</v>
       </c>
       <c r="E128" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>9439.8541580292003</v>
       </c>
       <c r="F128" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>113278.24989635037</v>
       </c>
       <c r="G128" s="16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>113.27824989635037</v>
       </c>
     </row>
@@ -4944,11 +5025,11 @@
         <v>25774</v>
       </c>
       <c r="E129" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>9439.8541580292003</v>
       </c>
       <c r="F129" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G129" s="16"/>
@@ -4964,11 +5045,11 @@
         <v>25774</v>
       </c>
       <c r="E130" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>9439.8541580292003</v>
       </c>
       <c r="F130" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G130" s="16"/>
@@ -4984,11 +5065,11 @@
         <v>25774</v>
       </c>
       <c r="E131" s="4">
-        <f t="shared" ref="E131:E139" si="14">500000/C131</f>
+        <f t="shared" ref="E131:E139" si="20">500000/C131</f>
         <v>9439.8541580292003</v>
       </c>
       <c r="F131" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G131" s="16"/>
@@ -5004,11 +5085,11 @@
         <v>25774</v>
       </c>
       <c r="E132" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>9439.8541580292003</v>
       </c>
       <c r="F132" s="4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G132" s="16"/>
@@ -5024,11 +5105,11 @@
         <v>25774</v>
       </c>
       <c r="E133" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>9439.8541580292003</v>
       </c>
       <c r="F133" s="4" t="str">
-        <f t="shared" ref="F133:F139" si="15">IF(D133=D132,"",SUMIF(D:D,D133,E:E))</f>
+        <f t="shared" ref="F133:F139" si="21">IF(D133=D132,"",SUMIF(D:D,D133,E:E))</f>
         <v/>
       </c>
       <c r="G133" s="16"/>
@@ -5044,11 +5125,11 @@
         <v>25774</v>
       </c>
       <c r="E134" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>9439.8541580292003</v>
       </c>
       <c r="F134" s="4" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="G134" s="16"/>
@@ -5064,11 +5145,11 @@
         <v>25774</v>
       </c>
       <c r="E135" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>9439.8541580292003</v>
       </c>
       <c r="F135" s="4" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="G135" s="16"/>
@@ -5084,11 +5165,11 @@
         <v>25774</v>
       </c>
       <c r="E136" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>9439.8541580292003</v>
       </c>
       <c r="F136" s="4" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="G136" s="16"/>
@@ -5104,11 +5185,11 @@
         <v>25774</v>
       </c>
       <c r="E137" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>9439.8541580292003</v>
       </c>
       <c r="F137" s="4" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="G137" s="16"/>
@@ -5124,11 +5205,11 @@
         <v>25774</v>
       </c>
       <c r="E138" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>9439.8541580292003</v>
       </c>
       <c r="F138" s="4" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="G138" s="16"/>
@@ -5144,11 +5225,11 @@
         <v>25774</v>
       </c>
       <c r="E139" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>9439.8541580292003</v>
       </c>
       <c r="F139" s="4" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="G139" s="16"/>

</xml_diff>